<commit_message>
Add method to Copy Clipboard data to one file, FYI DEF5138.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TestScripts.xlsx
+++ b/NformTester/NformTester/keywordscripts/TestScripts.xlsx
@@ -1259,7 +1259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7655" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7662" uniqueCount="885">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3964,6 +3964,21 @@
   </si>
   <si>
     <t>10.146.87.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CopyDataToFile</t>
+  </si>
+  <si>
+    <t>C:\Nform\user\CopyData.txt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"C:/Nform/user/CopyData.txt"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPS_10.146.83.20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4158,7 +4173,21 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4463,10 +4492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4680,7 +4709,7 @@
         <v>803</v>
       </c>
       <c r="B7" s="5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -5283,19 +5312,15 @@
         <v>836</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>802</v>
+        <v>881</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>880</v>
-      </c>
-      <c r="I27" s="3">
-        <v>1</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>879</v>
-      </c>
+        <v>882</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -5307,12 +5332,20 @@
       <c r="C28" s="3">
         <v>27</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="14" t="s">
+        <v>836</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>840</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>884</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -5325,13 +5358,23 @@
       <c r="C29" s="3">
         <v>28</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="14" t="s">
+        <v>836</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>802</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>879</v>
+      </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -5592,7 +5635,9 @@
     <row r="44" spans="1:14">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
-      <c r="C44" s="13"/>
+      <c r="C44" s="3">
+        <v>43</v>
+      </c>
       <c r="D44" s="14"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -5606,7 +5651,11 @@
       <c r="N44" s="4"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="C45" s="13"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="3">
+        <v>44</v>
+      </c>
       <c r="D45" s="14"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -5620,7 +5669,9 @@
       <c r="N45" s="4"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="C46" s="13"/>
+      <c r="C46" s="3">
+        <v>45</v>
+      </c>
       <c r="D46" s="14"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -5634,7 +5685,9 @@
       <c r="N46" s="4"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="C47" s="13"/>
+      <c r="C47" s="3">
+        <v>46</v>
+      </c>
       <c r="D47" s="14"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -5648,37 +5701,61 @@
       <c r="N47" s="4"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="C48" s="13"/>
+      <c r="C48" s="3">
+        <v>47</v>
+      </c>
       <c r="D48" s="14"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
       <c r="N48" s="4"/>
     </row>
-    <row r="49" spans="4:9">
+    <row r="49" spans="3:14">
+      <c r="C49" s="3">
+        <v>48</v>
+      </c>
       <c r="D49" s="14"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="13"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="4"/>
     </row>
-    <row r="50" spans="4:9">
-      <c r="D50" s="13"/>
+    <row r="50" spans="3:14">
+      <c r="C50" s="3">
+        <v>49</v>
+      </c>
+      <c r="D50" s="14"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="13"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="3:14">
+      <c r="C51" s="3">
+        <v>50</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N48">
+  <conditionalFormatting sqref="N2:N49">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
@@ -5687,16 +5764,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:D28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:D29">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 G13:G15 G7:G9 G11 G20:G50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5 G13:G15 G7:G9 G11 G20:G51">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12 F14:F15 F20:F50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12 F14:F15 F20:F51">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3 E8:E50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3 E8:E27 E29:E51">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix the problem for VerifyProperty
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TestScripts.xlsx
+++ b/NformTester/NformTester/keywordscripts/TestScripts.xlsx
@@ -1352,7 +1352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8244" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8173" uniqueCount="925">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4088,27 +4088,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>SingleManual</t>
-  </si>
-  <si>
-    <t>$SNMPdevice_0$</t>
-  </si>
-  <si>
-    <t>$GXT_0_NAME$</t>
-  </si>
-  <si>
-    <t>"Description for GXT"</t>
-  </si>
-  <si>
-    <t>"Liebert GXT UPS/WebCard"</t>
-  </si>
-  <si>
-    <t>"SNMP"</t>
-  </si>
-  <si>
     <t>No. Rows</t>
   </si>
   <si>
@@ -4119,17 +4098,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Result</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Enabled</t>
-  </si>
-  <si>
     <t>Exception / Error</t>
   </si>
   <si>
@@ -4139,15 +4111,9 @@
     <t>Ranorex Version</t>
   </si>
   <si>
-    <t>"action-one"</t>
-  </si>
-  <si>
     <t>Nform Viewer</t>
   </si>
   <si>
-    <t>"nform testing"</t>
-  </si>
-  <si>
     <t>Nform Server</t>
   </si>
   <si>
@@ -4160,35 +4126,39 @@
     <t>Managed device limit</t>
   </si>
   <si>
-    <t>"Run-command"</t>
-  </si>
-  <si>
     <t>Advanced Communications</t>
   </si>
   <si>
     <t>Advanced Notification</t>
   </si>
   <si>
-    <t>"C:\Nform\test.txt"</t>
-  </si>
-  <si>
     <t>Registration</t>
   </si>
   <si>
-    <t>"text"</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
-    <t>"2"</t>
-  </si>
-  <si>
     <t>.NET Framework</t>
   </si>
   <si>
-    <t>"{CONTROL down}{Akey}{CONTROL up}"</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <t>Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current devices: 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPS_10.146.82.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4401,21 +4371,7 @@
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="常规 2 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -4720,10 +4676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4735,7 +4691,7 @@
     <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25.5">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>878</v>
       </c>
@@ -4899,61 +4855,51 @@
       <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>903</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>701</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
+      <c r="D6" s="10" t="s">
         <v>904</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>905</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>906</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>907</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>908</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>909</v>
-      </c>
+      <c r="E6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>910</v>
+        <v>903</v>
       </c>
       <c r="B7" s="3">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4">
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>22</v>
+        <v>923</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -4961,29 +4907,33 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>912</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>913</v>
-      </c>
+        <v>905</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>19</v>
+        <v>695</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>80</v>
+        <v>699</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>921</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>922</v>
+      </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
@@ -4991,30 +4941,26 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4">
         <v>8</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>411</v>
+        <v>904</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>695</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>915</v>
-      </c>
-      <c r="I9" s="11" t="b">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -5023,27 +4969,35 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
-        <v>916</v>
+        <v>907</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>917</v>
+        <v>908</v>
       </c>
       <c r="C10" s="4">
         <v>9</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>899</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F10" s="11">
-        <v>5</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+        <v>904</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>633</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>921</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>924</v>
+      </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
@@ -5052,23 +5006,13 @@
     <row r="11" spans="1:14">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="4">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>411</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -5077,28 +5021,16 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="4">
-        <v>11</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>919</v>
-      </c>
-      <c r="I12" s="11"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -5107,27 +5039,15 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="18" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="4">
-        <v>12</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>921</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -5137,24 +5057,14 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="18" t="s">
-        <v>922</v>
+        <v>911</v>
       </c>
       <c r="B14" s="19"/>
-      <c r="C14" s="4">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="13"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -5165,26 +5075,16 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="18" t="s">
-        <v>923</v>
+        <v>912</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="C15" s="4">
-        <v>14</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
@@ -5193,26 +5093,16 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="18" t="s">
-        <v>924</v>
+        <v>913</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="C16" s="4">
-        <v>15</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
@@ -5221,28 +5111,16 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="18" t="s">
-        <v>925</v>
+        <v>914</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="4">
-        <v>16</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>926</v>
-      </c>
-      <c r="I17" s="13"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
@@ -5252,26 +5130,14 @@
     <row r="18" spans="1:14">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
-        <v>927</v>
-      </c>
-      <c r="C18" s="4">
-        <v>17</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>921</v>
-      </c>
+        <v>915</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
@@ -5282,26 +5148,14 @@
     <row r="19" spans="1:14">
       <c r="A19" s="18"/>
       <c r="B19" s="19" t="s">
-        <v>928</v>
-      </c>
-      <c r="C19" s="4">
-        <v>18</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>929</v>
-      </c>
+        <v>916</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -5311,29 +5165,17 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="18" t="s">
-        <v>930</v>
+        <v>917</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>917</v>
-      </c>
-      <c r="C20" s="4">
-        <v>19</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>463</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>931</v>
-      </c>
+        <v>908</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -5343,27 +5185,15 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="18" t="s">
-        <v>932</v>
+        <v>918</v>
       </c>
       <c r="B21" s="19"/>
-      <c r="C21" s="4">
-        <v>20</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>933</v>
-      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
@@ -5373,21 +5203,13 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="18" t="s">
-        <v>934</v>
+        <v>919</v>
       </c>
       <c r="B22" s="19"/>
-      <c r="C22" s="4">
-        <v>21</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>899</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F22" s="11">
-        <v>2</v>
-      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
@@ -5400,21 +5222,11 @@
     <row r="23" spans="1:14">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="4">
-        <v>22</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>461</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="11"/>
@@ -5426,18 +5238,10 @@
     <row r="24" spans="1:14">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="4">
-        <v>23</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>899</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>874</v>
-      </c>
-      <c r="F24" s="11">
-        <v>2</v>
-      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -5450,48 +5254,26 @@
     <row r="25" spans="1:14">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="4">
-        <v>24</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>696</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="11"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="C26" s="4">
-        <v>25</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>696</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>935</v>
-      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -5500,21 +5282,11 @@
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="C27" s="4">
-        <v>26</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>911</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -5523,27 +5295,37 @@
       <c r="M27" s="4"/>
       <c r="N27" s="6"/>
     </row>
+    <row r="28" spans="1:14">
+      <c r="C28" s="4"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N2:N27">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D4 D6:D28">
+      <formula1>"C,F,T,;"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F28">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G28">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D4 D6:D27">
-      <formula1>"C,F,T,;"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>